<commit_message>
Se hacen cambios al mostrar IDs no validos y ahora no se puede agregar dos empresas con el mismo nombre
</commit_message>
<xml_diff>
--- a/empresas.xlsx
+++ b/empresas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Nombre</t>
   </si>
@@ -25,16 +25,19 @@
     <t>Categoría</t>
   </si>
   <si>
+    <t>Zara</t>
+  </si>
+  <si>
+    <t>Empresa de ropa</t>
+  </si>
+  <si>
+    <t>Aleman</t>
+  </si>
+  <si>
     <t>Fanta</t>
   </si>
   <si>
     <t>Empresa de alimentos</t>
-  </si>
-  <si>
-    <t>Zara</t>
-  </si>
-  <si>
-    <t>Empresa de ropa</t>
   </si>
 </sst>
 </file>
@@ -411,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="4" width="25" customWidth="1"/>
@@ -436,10 +439,10 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -456,35 +459,21 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>